<commit_message>
Added test for reward function
</commit_message>
<xml_diff>
--- a/docs/QBEA.xlsx
+++ b/docs/QBEA.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Optimal" sheetId="3" r:id="rId1"/>
     <sheet name="Experiment" sheetId="4" r:id="rId2"/>
+    <sheet name="QBEA Q-Values" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
   <si>
     <t>Time</t>
   </si>
@@ -106,6 +107,24 @@
   </si>
   <si>
     <t>Time: 0.013 sec.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Running experiment QLearning bias: 100 repeated 1000 averaged over 1</t>
+  </si>
+  <si>
+    <t>Time: 0.043 sec.</t>
+  </si>
+  <si>
+    <t>Running experiment QBEA bias: 100 repeated 1000 averaged over 1</t>
+  </si>
+  <si>
+    <t>Time: 0.419 sec.</t>
+  </si>
+  <si>
+    <t>Time: 0.092 sec.</t>
   </si>
 </sst>
 </file>
@@ -490,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -2069,4 +2088,694 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>-10</v>
+      </c>
+      <c r="C2">
+        <v>-9</v>
+      </c>
+      <c r="D2">
+        <v>-8</v>
+      </c>
+      <c r="E2">
+        <v>-7</v>
+      </c>
+      <c r="F2">
+        <v>-6</v>
+      </c>
+      <c r="G2">
+        <v>-5</v>
+      </c>
+      <c r="H2">
+        <v>-4</v>
+      </c>
+      <c r="I2">
+        <v>-3</v>
+      </c>
+      <c r="J2">
+        <v>-2</v>
+      </c>
+      <c r="K2">
+        <v>-1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <v>7</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>9</v>
+      </c>
+      <c r="V2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>-5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>253.94</v>
+      </c>
+      <c r="D3">
+        <v>227.79</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>223.67</v>
+      </c>
+      <c r="G3">
+        <v>57.99</v>
+      </c>
+      <c r="H3">
+        <v>143.22999999999999</v>
+      </c>
+      <c r="I3">
+        <v>57.03</v>
+      </c>
+      <c r="J3">
+        <v>182.86</v>
+      </c>
+      <c r="K3">
+        <v>237.64</v>
+      </c>
+      <c r="L3">
+        <v>257.20999999999998</v>
+      </c>
+      <c r="M3">
+        <v>175.28</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>125.28</v>
+      </c>
+      <c r="P3">
+        <v>258.45</v>
+      </c>
+      <c r="Q3">
+        <v>172.87</v>
+      </c>
+      <c r="R3">
+        <v>249.84</v>
+      </c>
+      <c r="S3">
+        <v>214.91</v>
+      </c>
+      <c r="T3">
+        <v>271.81</v>
+      </c>
+      <c r="U3">
+        <v>335.57</v>
+      </c>
+      <c r="V3">
+        <v>212.57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>122.2</v>
+      </c>
+      <c r="C4">
+        <v>172.7</v>
+      </c>
+      <c r="D4">
+        <v>257.38</v>
+      </c>
+      <c r="E4">
+        <v>257.33999999999997</v>
+      </c>
+      <c r="F4">
+        <v>85.72</v>
+      </c>
+      <c r="G4">
+        <v>154.35</v>
+      </c>
+      <c r="H4">
+        <v>163.13999999999999</v>
+      </c>
+      <c r="I4">
+        <v>128.41999999999999</v>
+      </c>
+      <c r="J4">
+        <v>236.73</v>
+      </c>
+      <c r="K4">
+        <v>273.25</v>
+      </c>
+      <c r="L4">
+        <v>112.09</v>
+      </c>
+      <c r="M4">
+        <v>272.23</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>155.28</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>258.64</v>
+      </c>
+      <c r="R4">
+        <v>344.9</v>
+      </c>
+      <c r="S4">
+        <v>106.96</v>
+      </c>
+      <c r="T4">
+        <v>247.98</v>
+      </c>
+      <c r="U4">
+        <v>33.21</v>
+      </c>
+      <c r="V4">
+        <v>141.80000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>102200</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>-10</v>
+      </c>
+      <c r="C8">
+        <v>-9</v>
+      </c>
+      <c r="D8">
+        <v>-8</v>
+      </c>
+      <c r="E8">
+        <v>-7</v>
+      </c>
+      <c r="F8">
+        <v>-6</v>
+      </c>
+      <c r="G8">
+        <v>-5</v>
+      </c>
+      <c r="H8">
+        <v>-4</v>
+      </c>
+      <c r="I8">
+        <v>-3</v>
+      </c>
+      <c r="J8">
+        <v>-2</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <v>8</v>
+      </c>
+      <c r="U8">
+        <v>9</v>
+      </c>
+      <c r="V8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>-5</v>
+      </c>
+      <c r="B9">
+        <v>145.11000000000001</v>
+      </c>
+      <c r="C9">
+        <v>147.13999999999999</v>
+      </c>
+      <c r="D9">
+        <v>149.11000000000001</v>
+      </c>
+      <c r="E9">
+        <v>151.11000000000001</v>
+      </c>
+      <c r="F9">
+        <v>153.1</v>
+      </c>
+      <c r="G9">
+        <v>156.41</v>
+      </c>
+      <c r="H9">
+        <v>153.09</v>
+      </c>
+      <c r="I9">
+        <v>151.27000000000001</v>
+      </c>
+      <c r="J9">
+        <v>149.15</v>
+      </c>
+      <c r="K9">
+        <v>147.11000000000001</v>
+      </c>
+      <c r="L9">
+        <v>145.11000000000001</v>
+      </c>
+      <c r="M9">
+        <v>143.11000000000001</v>
+      </c>
+      <c r="N9">
+        <v>141.11000000000001</v>
+      </c>
+      <c r="O9">
+        <v>139.11000000000001</v>
+      </c>
+      <c r="P9">
+        <v>137.11000000000001</v>
+      </c>
+      <c r="Q9">
+        <v>135.11000000000001</v>
+      </c>
+      <c r="R9">
+        <v>133.11000000000001</v>
+      </c>
+      <c r="S9">
+        <v>131.11000000000001</v>
+      </c>
+      <c r="T9">
+        <v>129.11000000000001</v>
+      </c>
+      <c r="U9">
+        <v>127.11</v>
+      </c>
+      <c r="V9">
+        <v>125.11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>7.29</v>
+      </c>
+      <c r="C10">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="D10">
+        <v>11.29</v>
+      </c>
+      <c r="E10">
+        <v>13.29</v>
+      </c>
+      <c r="F10">
+        <v>15.29</v>
+      </c>
+      <c r="G10">
+        <v>17.29</v>
+      </c>
+      <c r="H10">
+        <v>19.29</v>
+      </c>
+      <c r="I10">
+        <v>21.29</v>
+      </c>
+      <c r="J10">
+        <v>23.29</v>
+      </c>
+      <c r="K10">
+        <v>25.29</v>
+      </c>
+      <c r="L10">
+        <v>27.29</v>
+      </c>
+      <c r="M10">
+        <v>29.29</v>
+      </c>
+      <c r="N10">
+        <v>-58.79</v>
+      </c>
+      <c r="O10">
+        <v>33.29</v>
+      </c>
+      <c r="P10">
+        <v>35.28</v>
+      </c>
+      <c r="Q10">
+        <v>38.54</v>
+      </c>
+      <c r="R10">
+        <v>35.590000000000003</v>
+      </c>
+      <c r="S10">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="T10">
+        <v>31.29</v>
+      </c>
+      <c r="U10">
+        <v>29.29</v>
+      </c>
+      <c r="V10">
+        <v>27.29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>25436</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>-10</v>
+      </c>
+      <c r="C16">
+        <v>-9</v>
+      </c>
+      <c r="D16">
+        <v>-8</v>
+      </c>
+      <c r="E16">
+        <v>-7</v>
+      </c>
+      <c r="F16">
+        <v>-6</v>
+      </c>
+      <c r="G16">
+        <v>-5</v>
+      </c>
+      <c r="H16">
+        <v>-4</v>
+      </c>
+      <c r="I16">
+        <v>-3</v>
+      </c>
+      <c r="J16">
+        <v>-2</v>
+      </c>
+      <c r="K16">
+        <v>-1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <v>7</v>
+      </c>
+      <c r="T16">
+        <v>8</v>
+      </c>
+      <c r="U16">
+        <v>9</v>
+      </c>
+      <c r="V16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>-5</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>253.94</v>
+      </c>
+      <c r="D17">
+        <v>227.79</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>223.67</v>
+      </c>
+      <c r="G17">
+        <v>57.99</v>
+      </c>
+      <c r="H17">
+        <v>143.22999999999999</v>
+      </c>
+      <c r="I17">
+        <v>57.03</v>
+      </c>
+      <c r="J17">
+        <v>182.86</v>
+      </c>
+      <c r="K17">
+        <v>237.64</v>
+      </c>
+      <c r="L17">
+        <v>257.20999999999998</v>
+      </c>
+      <c r="M17">
+        <v>175.28</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>125.28</v>
+      </c>
+      <c r="P17">
+        <v>258.45</v>
+      </c>
+      <c r="Q17">
+        <v>172.87</v>
+      </c>
+      <c r="R17">
+        <v>249.84</v>
+      </c>
+      <c r="S17">
+        <v>214.91</v>
+      </c>
+      <c r="T17">
+        <v>271.81</v>
+      </c>
+      <c r="U17">
+        <v>335.57</v>
+      </c>
+      <c r="V17">
+        <v>212.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>122.2</v>
+      </c>
+      <c r="C18">
+        <v>172.7</v>
+      </c>
+      <c r="D18">
+        <v>257.38</v>
+      </c>
+      <c r="E18">
+        <v>257.33999999999997</v>
+      </c>
+      <c r="F18">
+        <v>85.72</v>
+      </c>
+      <c r="G18">
+        <v>154.35</v>
+      </c>
+      <c r="H18">
+        <v>163.13999999999999</v>
+      </c>
+      <c r="I18">
+        <v>128.41999999999999</v>
+      </c>
+      <c r="J18">
+        <v>236.73</v>
+      </c>
+      <c r="K18">
+        <v>273.25</v>
+      </c>
+      <c r="L18">
+        <v>112.09</v>
+      </c>
+      <c r="M18">
+        <v>272.23</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>155.28</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>258.64</v>
+      </c>
+      <c r="R18">
+        <v>344.9</v>
+      </c>
+      <c r="S18">
+        <v>106.96</v>
+      </c>
+      <c r="T18">
+        <v>247.98</v>
+      </c>
+      <c r="U18">
+        <v>33.21</v>
+      </c>
+      <c r="V18">
+        <v>141.80000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>102200</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 1+1 Strategy to EDOAlgorithm Changed Experiment to pass in a LearningAlgorithm
</commit_message>
<xml_diff>
--- a/docs/QBEA.xlsx
+++ b/docs/QBEA.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EDO Strategies 100" sheetId="13" r:id="rId1"/>
-    <sheet name="EDO Strategies 15" sheetId="15" r:id="rId2"/>
-    <sheet name="Results t=0" sheetId="9" r:id="rId3"/>
-    <sheet name="Results ft" sheetId="11" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId5"/>
-    <sheet name="Vary bias" sheetId="6" r:id="rId6"/>
-    <sheet name="Optimal" sheetId="3" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="16" r:id="rId2"/>
+    <sheet name="EDO Strategies 15" sheetId="15" r:id="rId3"/>
+    <sheet name="Results t=0" sheetId="9" r:id="rId4"/>
+    <sheet name="Results ft" sheetId="11" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId6"/>
+    <sheet name="Vary bias" sheetId="6" r:id="rId7"/>
+    <sheet name="Optimal" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="71">
   <si>
     <t>Time</t>
   </si>
@@ -231,6 +232,18 @@
   </si>
   <si>
     <t>QBEA:</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>Random then best</t>
+  </si>
+  <si>
+    <t>RTB - 1+1</t>
+  </si>
+  <si>
+    <t>Split</t>
   </si>
 </sst>
 </file>
@@ -11165,7 +11178,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11630,7 +11642,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11737,7 +11748,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12202,7 +12212,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12309,7 +12318,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12774,7 +12782,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12881,7 +12888,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13346,7 +13352,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13453,7 +13458,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14507,7 +14511,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14614,7 +14617,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15247,7 +15249,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15354,7 +15355,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15987,7 +15987,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16094,7 +16093,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17039,7 +17037,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17146,7 +17143,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18091,7 +18087,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18198,7 +18193,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19743,7 +19737,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19850,7 +19843,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21395,7 +21387,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -37539,7 +37530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -38984,6 +38975,1167 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>22209.0666666666</v>
+      </c>
+      <c r="C3" s="5">
+        <v>22209.0666666666</v>
+      </c>
+      <c r="D3" s="5">
+        <f>C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>17806.0666666666</v>
+      </c>
+      <c r="H3" s="5">
+        <v>17806.0666666666</v>
+      </c>
+      <c r="I3" s="5">
+        <f>H3-G3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>22209.0666666666</v>
+      </c>
+      <c r="C4" s="5">
+        <v>22209.0666666666</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:D24" si="0">C4-B4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>17806.0666666666</v>
+      </c>
+      <c r="H4" s="5">
+        <v>17806.0666666666</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" ref="I4:I24" si="1">H4-G4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>27359.5333333333</v>
+      </c>
+      <c r="C5" s="5">
+        <v>28046.933333333302</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>687.40000000000146</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5">
+        <v>22996.2</v>
+      </c>
+      <c r="H5" s="5">
+        <v>23014.933333333302</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="1"/>
+        <v>18.733333333300834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>28649.933333333302</v>
+      </c>
+      <c r="C6" s="5">
+        <v>28642.733333333301</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>-7.2000000000007276</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>25096.933333333302</v>
+      </c>
+      <c r="H6" s="5">
+        <v>25021.733333333301</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="1"/>
+        <v>-75.200000000000728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>28597.4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>29236.6</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>639.19999999999709</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
+        <v>26177.733333333301</v>
+      </c>
+      <c r="H7" s="5">
+        <v>26176.6</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.1333333333022892</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5">
+        <v>28577.866666666599</v>
+      </c>
+      <c r="C8" s="5">
+        <v>28821.200000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>243.33333333340124</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>26804.2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>26735.866666666599</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="1"/>
+        <v>-68.333333333401242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
+        <v>28336.733333333301</v>
+      </c>
+      <c r="C9" s="5">
+        <v>28573.733333333301</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>237</v>
+      </c>
+      <c r="F9" s="5">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5">
+        <v>27231.733333333301</v>
+      </c>
+      <c r="H9" s="5">
+        <v>27123.0666666666</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="1"/>
+        <v>-108.66666666670062</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>28347.4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>28579.200000000001</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>231.79999999999927</v>
+      </c>
+      <c r="F10" s="5">
+        <v>7</v>
+      </c>
+      <c r="G10" s="5">
+        <v>27582.400000000001</v>
+      </c>
+      <c r="H10" s="5">
+        <v>27496.866666666599</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="1"/>
+        <v>-85.53333333340197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5">
+        <v>28408.5333333333</v>
+      </c>
+      <c r="C11" s="5">
+        <v>28471.599999999999</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>63.066666666698438</v>
+      </c>
+      <c r="F11" s="5">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5">
+        <v>27819.200000000001</v>
+      </c>
+      <c r="H11" s="5">
+        <v>27740.6</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="1"/>
+        <v>-78.600000000002183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>28403.266666666601</v>
+      </c>
+      <c r="C12" s="5">
+        <v>28378.0666666666</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.200000000000728</v>
+      </c>
+      <c r="F12" s="5">
+        <v>9</v>
+      </c>
+      <c r="G12" s="5">
+        <v>28023.599999999999</v>
+      </c>
+      <c r="H12" s="5">
+        <v>27902.0666666666</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="1"/>
+        <v>-121.53333333339833</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>28503.133333333299</v>
+      </c>
+      <c r="C13" s="5">
+        <v>28533.599999999999</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>30.466666666699894</v>
+      </c>
+      <c r="F13" s="5">
+        <v>10</v>
+      </c>
+      <c r="G13" s="5">
+        <v>28208.466666666602</v>
+      </c>
+      <c r="H13" s="5">
+        <v>28142.6</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="1"/>
+        <v>-65.866666666603123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5">
+        <v>28591.4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>28539.8</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>-51.600000000002183</v>
+      </c>
+      <c r="F14" s="5">
+        <v>11</v>
+      </c>
+      <c r="G14" s="5">
+        <v>28364.733333333301</v>
+      </c>
+      <c r="H14" s="5">
+        <v>28262.133333333299</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="1"/>
+        <v>-102.60000000000218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5">
+        <v>28738.933333333302</v>
+      </c>
+      <c r="C15" s="5">
+        <v>28655.599999999999</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>-83.333333333303017</v>
+      </c>
+      <c r="F15" s="5">
+        <v>12</v>
+      </c>
+      <c r="G15" s="5">
+        <v>28506.6</v>
+      </c>
+      <c r="H15" s="5">
+        <v>28411.933333333302</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="1"/>
+        <v>-94.666666666696983</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5">
+        <v>28819.5333333333</v>
+      </c>
+      <c r="C16" s="5">
+        <v>28752.6</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>-66.933333333301562</v>
+      </c>
+      <c r="F16" s="5">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5">
+        <v>28621.200000000001</v>
+      </c>
+      <c r="H16" s="5">
+        <v>28542.933333333302</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="1"/>
+        <v>-78.266666666699166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5">
+        <v>28912.933333333302</v>
+      </c>
+      <c r="C17" s="5">
+        <v>28815.466666666602</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>-97.466666666699894</v>
+      </c>
+      <c r="F17" s="5">
+        <v>14</v>
+      </c>
+      <c r="G17" s="5">
+        <v>28737.266666666601</v>
+      </c>
+      <c r="H17" s="5">
+        <v>28622.799999999999</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="1"/>
+        <v>-114.46666666660167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5">
+        <v>29021.866666666599</v>
+      </c>
+      <c r="C18" s="5">
+        <v>28937.4</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>-84.46666666659803</v>
+      </c>
+      <c r="F18" s="5">
+        <v>15</v>
+      </c>
+      <c r="G18" s="5">
+        <v>28834.866666666599</v>
+      </c>
+      <c r="H18" s="5">
+        <v>28744.733333333301</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="1"/>
+        <v>-90.133333333298651</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5">
+        <v>29090.466666666602</v>
+      </c>
+      <c r="C19" s="5">
+        <v>29000.866666666599</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>-89.600000000002183</v>
+      </c>
+      <c r="F19" s="5">
+        <v>16</v>
+      </c>
+      <c r="G19" s="5">
+        <v>28914.799999999999</v>
+      </c>
+      <c r="H19" s="5">
+        <v>28825.200000000001</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="1"/>
+        <v>-89.599999999998545</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5">
+        <v>29164.2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>29090.5333333333</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>-73.666666666700621</v>
+      </c>
+      <c r="F20" s="5">
+        <v>17</v>
+      </c>
+      <c r="G20" s="5">
+        <v>28988.5333333333</v>
+      </c>
+      <c r="H20" s="5">
+        <v>28909.200000000001</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" si="1"/>
+        <v>-79.333333333299379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5">
+        <v>29230.733333333301</v>
+      </c>
+      <c r="C21" s="5">
+        <v>29141.4</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>-89.333333333299379</v>
+      </c>
+      <c r="F21" s="5">
+        <v>18</v>
+      </c>
+      <c r="G21" s="5">
+        <v>29055.0666666666</v>
+      </c>
+      <c r="H21" s="5">
+        <v>28965.733333333301</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="1"/>
+        <v>-89.333333333299379</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5">
+        <v>29279.8</v>
+      </c>
+      <c r="C22" s="5">
+        <v>29203.4</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>-76.399999999997817</v>
+      </c>
+      <c r="F22" s="5">
+        <v>19</v>
+      </c>
+      <c r="G22" s="5">
+        <v>29109.8</v>
+      </c>
+      <c r="H22" s="5">
+        <v>29027.733333333301</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" si="1"/>
+        <v>-82.066666666698438</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5">
+        <v>29354.266666666601</v>
+      </c>
+      <c r="C23" s="5">
+        <v>29264.6</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>-89.666666666602396</v>
+      </c>
+      <c r="F23" s="5">
+        <v>20</v>
+      </c>
+      <c r="G23" s="5">
+        <v>29184.266666666601</v>
+      </c>
+      <c r="H23" s="5">
+        <v>29088.933333333302</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="1"/>
+        <v>-95.333333333299379</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>21</v>
+      </c>
+      <c r="B24" s="5">
+        <v>30200</v>
+      </c>
+      <c r="C24" s="5">
+        <v>30200</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>21</v>
+      </c>
+      <c r="G24" s="5">
+        <v>30030</v>
+      </c>
+      <c r="H24" s="5">
+        <v>30030</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="5">
+        <v>117632.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28">
+        <v>32712.5333333333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>116979.8</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>32099.4</v>
+      </c>
+      <c r="H30">
+        <v>32612.333333333299</v>
+      </c>
+      <c r="I30">
+        <v>32294.333333333299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>22433.5333333333</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>17894.5333333333</v>
+      </c>
+      <c r="H31">
+        <v>32242.466666666602</v>
+      </c>
+      <c r="I31">
+        <v>31403.666666666599</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>117004.33333333299</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>32190.0666666666</v>
+      </c>
+      <c r="H32">
+        <v>31940.2</v>
+      </c>
+      <c r="I32">
+        <v>31596.733333333301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>116984.8</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <v>31737.5333333333</v>
+      </c>
+      <c r="H33">
+        <v>31755.266666666601</v>
+      </c>
+      <c r="I33">
+        <v>31037.5333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>116545.2</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>31167.866666666599</v>
+      </c>
+      <c r="H34">
+        <v>31453.5333333333</v>
+      </c>
+      <c r="I34">
+        <v>32670.5333333333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>116328.066666666</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>31820.400000000001</v>
+      </c>
+      <c r="H35">
+        <v>32139.200000000001</v>
+      </c>
+      <c r="I35">
+        <v>31597.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>117539.33333333299</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>32647.4</v>
+      </c>
+      <c r="H36">
+        <v>31566.266666666601</v>
+      </c>
+      <c r="I36">
+        <v>31406.733333333301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <v>117311.33333333299</v>
+      </c>
+      <c r="F37">
+        <v>7</v>
+      </c>
+      <c r="G37">
+        <v>31254.0666666666</v>
+      </c>
+      <c r="H37">
+        <v>32007.666666666599</v>
+      </c>
+      <c r="I37">
+        <v>32656.666666666599</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>116986.933333333</v>
+      </c>
+      <c r="F38">
+        <v>8</v>
+      </c>
+      <c r="G38">
+        <v>32560.866666666599</v>
+      </c>
+      <c r="H38">
+        <v>32340.333333333299</v>
+      </c>
+      <c r="I38">
+        <v>31184.933333333302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>117794.8</v>
+      </c>
+      <c r="F39">
+        <v>9</v>
+      </c>
+      <c r="G39">
+        <v>33037.800000000003</v>
+      </c>
+      <c r="H39">
+        <v>32099.5333333333</v>
+      </c>
+      <c r="I39">
+        <v>31811.333333333299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>117677.33333333299</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>32348.5333333333</v>
+      </c>
+      <c r="H40">
+        <v>31395.933333333302</v>
+      </c>
+      <c r="I40">
+        <v>31256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>116952.866666666</v>
+      </c>
+      <c r="F41">
+        <v>11</v>
+      </c>
+      <c r="G41">
+        <v>32277.599999999999</v>
+      </c>
+      <c r="H41">
+        <v>32458.133333333299</v>
+      </c>
+      <c r="I41">
+        <v>32918</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <v>116780.933333333</v>
+      </c>
+      <c r="F42">
+        <v>12</v>
+      </c>
+      <c r="G42">
+        <v>32177.5333333333</v>
+      </c>
+      <c r="H42">
+        <v>32184.0666666666</v>
+      </c>
+      <c r="I42">
+        <v>31114.133333333299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>13</v>
+      </c>
+      <c r="B43">
+        <v>116568.6</v>
+      </c>
+      <c r="F43">
+        <v>13</v>
+      </c>
+      <c r="G43">
+        <v>32217.733333333301</v>
+      </c>
+      <c r="H43">
+        <v>32317.200000000001</v>
+      </c>
+      <c r="I43">
+        <v>32406.733333333301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>117198.26666666599</v>
+      </c>
+      <c r="F44">
+        <v>14</v>
+      </c>
+      <c r="G44">
+        <v>34504.466666666602</v>
+      </c>
+      <c r="H44">
+        <v>33005.933333333298</v>
+      </c>
+      <c r="I44">
+        <v>31732.933333333302</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>117599.8</v>
+      </c>
+      <c r="F45">
+        <v>15</v>
+      </c>
+      <c r="G45">
+        <v>33008.400000000001</v>
+      </c>
+      <c r="H45">
+        <v>32367.599999999999</v>
+      </c>
+      <c r="I45">
+        <v>31921.0666666666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>117154.933333333</v>
+      </c>
+      <c r="F46">
+        <v>16</v>
+      </c>
+      <c r="G46">
+        <v>32903.933333333298</v>
+      </c>
+      <c r="H46">
+        <v>32716.466666666602</v>
+      </c>
+      <c r="I46">
+        <v>32278.266666666601</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <v>118157.6</v>
+      </c>
+      <c r="F47">
+        <v>17</v>
+      </c>
+      <c r="G47">
+        <v>33024.199999999997</v>
+      </c>
+      <c r="H47">
+        <v>32144.0666666666</v>
+      </c>
+      <c r="I47">
+        <v>32325.666666666599</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>117031.666666666</v>
+      </c>
+      <c r="F48">
+        <v>18</v>
+      </c>
+      <c r="G48">
+        <v>33959.133333333302</v>
+      </c>
+      <c r="H48">
+        <v>32817.266666666597</v>
+      </c>
+      <c r="I48">
+        <v>32586.333333333299</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>19</v>
+      </c>
+      <c r="B49">
+        <v>117943.8</v>
+      </c>
+      <c r="F49">
+        <v>19</v>
+      </c>
+      <c r="G49">
+        <v>33736.400000000001</v>
+      </c>
+      <c r="H49">
+        <v>31875.0666666666</v>
+      </c>
+      <c r="I49">
+        <v>32651.666666666599</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>117401.33333333299</v>
+      </c>
+      <c r="F50">
+        <v>20</v>
+      </c>
+      <c r="G50">
+        <v>33162.266666666597</v>
+      </c>
+      <c r="H50">
+        <v>32051.4</v>
+      </c>
+      <c r="I50">
+        <v>32041.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <v>116295.933333333</v>
+      </c>
+      <c r="F51">
+        <v>21</v>
+      </c>
+      <c r="G51">
+        <v>32918.6</v>
+      </c>
+      <c r="H51">
+        <v>32182.666666666599</v>
+      </c>
+      <c r="I51">
+        <v>32608.400000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N74"/>
   <sheetViews>
@@ -40838,7 +41990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:CX64"/>
   <sheetViews>
@@ -45619,7 +46771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI110"/>
   <sheetViews>
@@ -48272,7 +49424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L76"/>
   <sheetViews>
@@ -49981,7 +51133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -50192,7 +51344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>

</xml_diff>